<commit_message>
TODO: revise the last worksheet analysis and add a graphic to visualize it
</commit_message>
<xml_diff>
--- a/analysis/Transfers Analysis.xlsx
+++ b/analysis/Transfers Analysis.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/d04025c766eef03f/workspace/365DataScience-Excel-FootballTransfersAnalysis/analysis/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="486" documentId="11_F25DC773A252ABDACC10485C419873D45ADE58EE" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{EC58710D-33FB-4F4D-A720-91F6AB4FF240}"/>
+  <xr:revisionPtr revIDLastSave="488" documentId="11_F25DC773A252ABDACC10485C419873D45ADE58EE" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9E466348-994D-40CB-B583-C4B2C966D7FB}"/>
   <bookViews>
-    <workbookView xWindow="3000" yWindow="2865" windowWidth="21600" windowHeight="11835" firstSheet="2" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3825" yWindow="1905" windowWidth="21600" windowHeight="11835" firstSheet="2" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="_database" sheetId="5" state="hidden" r:id="rId1"/>
@@ -78,7 +78,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17112" uniqueCount="179">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17113" uniqueCount="180">
   <si>
     <t>Analyze European Transfers</t>
   </si>
@@ -687,6 +687,9 @@
     <t>2022/2023
 Total $ / Total #</t>
   </si>
+  <si>
+    <t>// TODO: revise it and add a graphic to visualize it</t>
+  </si>
 </sst>
 </file>
 
@@ -79505,7 +79508,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{022D8DCC-B36E-4D1B-A09D-6942F643F097}">
   <dimension ref="B1:O48"/>
   <sheetViews>
-    <sheetView showGridLines="0" showRowColHeaders="0" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView showGridLines="0" showRowColHeaders="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="L4" activeCellId="1" sqref="I4 L4"/>
       <extLst>
         <ext xmlns:xlsdti="http://schemas.microsoft.com/office/spreadsheetml/2023/showDataTypeIcons" uri="{77bfe23e-c014-4d31-8a63-9c772dbf06b6}">
@@ -82068,6 +82071,7 @@
       </c>
     </row>
   </sheetData>
+  <sheetProtection sheet="1" objects="1" scenarios="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -82075,10 +82079,10 @@
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BC8D4B04-5487-43ED-BA04-3B1233473CE4}">
   <sheetPr filterMode="1"/>
-  <dimension ref="B1:E48"/>
+  <dimension ref="B1:E50"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B51" sqref="B51"/>
+    <sheetView topLeftCell="A24" workbookViewId="0">
+      <selection activeCell="B50" sqref="B50"/>
       <extLst>
         <ext xmlns:xlsdti="http://schemas.microsoft.com/office/spreadsheetml/2023/showDataTypeIcons" uri="{77bfe23e-c014-4d31-8a63-9c772dbf06b6}">
           <xlsdti:showDataTypeIcons visible="0"/>
@@ -82717,6 +82721,11 @@
       </c>
       <c r="D48" t="s">
         <v>154</v>
+      </c>
+    </row>
+    <row r="50" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B50" t="s">
+        <v>179</v>
       </c>
     </row>
   </sheetData>

</xml_diff>